<commit_message>
Updated Home Page and Added Best.mp4
</commit_message>
<xml_diff>
--- a/Romi Pins.xlsx
+++ b/Romi Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/clbonney_calpoly_edu/Documents/ME 405 Mechatronics Lab/ME405-Mechatronics-Romi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2052" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23BED8FB-D14D-4848-A900-B4A0927756E0}"/>
+  <xr:revisionPtr revIDLastSave="2054" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B08F6418-2903-4CDA-8D0C-2C6AF8759B07}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19380" xr2:uid="{2EB5B3E0-4CA6-4DEA-8D58-C3FD12820291}"/>
+    <workbookView minimized="1" xWindow="1170" yWindow="0" windowWidth="26010" windowHeight="20880" activeTab="1" xr2:uid="{2EB5B3E0-4CA6-4DEA-8D58-C3FD12820291}"/>
   </bookViews>
   <sheets>
     <sheet name="Nucleo_Pinout_Table" sheetId="5" r:id="rId1"/>
@@ -1478,128 +1478,7 @@
       </font>
       <fill>
         <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.749961851863155"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1732,6 +1611,127 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1938,8 +1938,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="22883567" y="1520054"/>
-          <a:ext cx="7557883" cy="1607461"/>
+          <a:off x="20066374" y="1514475"/>
+          <a:ext cx="6667523" cy="1600287"/>
           <a:chOff x="11820145" y="6660710"/>
           <a:chExt cx="6630544" cy="1835997"/>
         </a:xfrm>
@@ -2749,35 +2749,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0FF3C0-CECB-2D4C-9343-7B8484A1E447}">
   <dimension ref="B2:AL158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM4" zoomScale="239" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AV21" sqref="AV21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="18" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="18" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="18.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="18"/>
+    <col min="11" max="11" width="17.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="18" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="76"/>
     </row>
-    <row r="3" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="76">
         <f>ROW()-ROW($B$2)</f>
         <v>1</v>
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="76">
         <f>ROW()-ROW($B$2)</f>
         <v>2</v>
@@ -2795,7 +2795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="76">
         <f>ROW()-ROW($B$2)</f>
         <v>3</v>
@@ -2804,7 +2804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="82" t="s">
         <v>4</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="AK7" s="87"/>
       <c r="AL7" s="88"/>
     </row>
-    <row r="8" spans="2:38" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:38" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="36" t="s">
         <v>8</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="AK8" s="59"/>
       <c r="AL8" s="60"/>
     </row>
-    <row r="9" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>14</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="AK9" s="59"/>
       <c r="AL9" s="60"/>
     </row>
-    <row r="10" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>14</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="AK10" s="59"/>
       <c r="AL10" s="60"/>
     </row>
-    <row r="11" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
@@ -3065,7 +3065,7 @@
       <c r="AK11" s="59"/>
       <c r="AL11" s="60"/>
     </row>
-    <row r="12" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3113,7 +3113,7 @@
       <c r="AK12" s="59"/>
       <c r="AL12" s="60"/>
     </row>
-    <row r="13" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27" t="s">
         <v>41</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="AK13" s="59"/>
       <c r="AL13" s="60"/>
     </row>
-    <row r="14" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
         <v>41</v>
       </c>
@@ -3221,7 +3221,7 @@
       <c r="AK14" s="59"/>
       <c r="AL14" s="60"/>
     </row>
-    <row r="15" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
         <v>46</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="AK15" s="59"/>
       <c r="AL15" s="60"/>
     </row>
-    <row r="16" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27" t="s">
         <v>46</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="AK16" s="62"/>
       <c r="AL16" s="63"/>
     </row>
-    <row r="17" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>31</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="X17" s="39"/>
       <c r="Y17" s="40"/>
     </row>
-    <row r="18" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
@@ -3413,7 +3413,7 @@
       <c r="AK18" s="87"/>
       <c r="AL18" s="88"/>
     </row>
-    <row r="19" spans="2:38" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:38" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
         <v>30</v>
       </c>
@@ -3471,7 +3471,7 @@
       <c r="AK19" s="59"/>
       <c r="AL19" s="60"/>
     </row>
-    <row r="20" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
         <v>46</v>
       </c>
@@ -3527,7 +3527,7 @@
       <c r="AK20" s="59"/>
       <c r="AL20" s="60"/>
     </row>
-    <row r="21" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
         <v>46</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="AK21" s="59"/>
       <c r="AL21" s="60"/>
     </row>
-    <row r="22" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>46</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="AK22" s="59"/>
       <c r="AL22" s="60"/>
     </row>
-    <row r="23" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>50</v>
       </c>
@@ -3685,7 +3685,7 @@
       <c r="AK23" s="59"/>
       <c r="AL23" s="60"/>
     </row>
-    <row r="24" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>61</v>
       </c>
@@ -3736,7 +3736,7 @@
       <c r="AK24" s="59"/>
       <c r="AL24" s="60"/>
     </row>
-    <row r="25" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -3781,7 +3781,7 @@
       <c r="AK25" s="59"/>
       <c r="AL25" s="60"/>
     </row>
-    <row r="26" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
@@ -3828,7 +3828,7 @@
       <c r="AK26" s="59"/>
       <c r="AL26" s="60"/>
     </row>
-    <row r="27" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="28" t="s">
         <v>55</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="AK27" s="59"/>
       <c r="AL27" s="60"/>
     </row>
-    <row r="28" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O28" s="38"/>
       <c r="P28" s="39"/>
       <c r="Q28" s="39"/>
@@ -3906,7 +3906,7 @@
       <c r="AK28" s="59"/>
       <c r="AL28" s="60"/>
     </row>
-    <row r="29" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="82" t="s">
         <v>103</v>
       </c>
@@ -3945,7 +3945,7 @@
       <c r="AK29" s="59"/>
       <c r="AL29" s="60"/>
     </row>
-    <row r="30" spans="2:38" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:38" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36" t="s">
         <v>8</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="AK30" s="59"/>
       <c r="AL30" s="60"/>
     </row>
-    <row r="31" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
         <v>20</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="AK31" s="59"/>
       <c r="AL31" s="60"/>
     </row>
-    <row r="32" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="27" t="s">
         <v>14</v>
       </c>
@@ -4090,7 +4090,7 @@
       <c r="AK32" s="59"/>
       <c r="AL32" s="60"/>
     </row>
-    <row r="33" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
@@ -4135,7 +4135,7 @@
       <c r="AK33" s="59"/>
       <c r="AL33" s="60"/>
     </row>
-    <row r="34" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
@@ -4174,7 +4174,7 @@
       <c r="AK34" s="59"/>
       <c r="AL34" s="60"/>
     </row>
-    <row r="35" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
@@ -4221,7 +4221,7 @@
       <c r="AK35" s="59"/>
       <c r="AL35" s="60"/>
     </row>
-    <row r="36" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
         <v>46</v>
       </c>
@@ -4270,7 +4270,7 @@
       <c r="AK36" s="59"/>
       <c r="AL36" s="60"/>
     </row>
-    <row r="37" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>50</v>
       </c>
@@ -4319,7 +4319,7 @@
       <c r="AK37" s="59"/>
       <c r="AL37" s="60"/>
     </row>
-    <row r="38" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
         <v>61</v>
       </c>
@@ -4364,7 +4364,7 @@
       <c r="AK38" s="59"/>
       <c r="AL38" s="60"/>
     </row>
-    <row r="39" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="27" t="s">
         <v>30</v>
       </c>
@@ -4417,7 +4417,7 @@
       <c r="AK39" s="59"/>
       <c r="AL39" s="60"/>
     </row>
-    <row r="40" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="27" t="s">
         <v>31</v>
       </c>
@@ -4468,7 +4468,7 @@
       <c r="AK40" s="59"/>
       <c r="AL40" s="60"/>
     </row>
-    <row r="41" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="27" t="s">
         <v>46</v>
       </c>
@@ -4517,7 +4517,7 @@
       <c r="AK41" s="59"/>
       <c r="AL41" s="60"/>
     </row>
-    <row r="42" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
@@ -4562,7 +4562,7 @@
       <c r="AK42" s="59"/>
       <c r="AL42" s="60"/>
     </row>
-    <row r="43" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
         <v>37</v>
       </c>
@@ -4607,7 +4607,7 @@
       <c r="AK43" s="59"/>
       <c r="AL43" s="60"/>
     </row>
-    <row r="44" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="27" t="s">
         <v>61</v>
       </c>
@@ -4654,7 +4654,7 @@
       <c r="AK44" s="59"/>
       <c r="AL44" s="60"/>
     </row>
-    <row r="45" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
         <v>50</v>
       </c>
@@ -4701,7 +4701,7 @@
       <c r="AK45" s="59"/>
       <c r="AL45" s="60"/>
     </row>
-    <row r="46" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -4740,7 +4740,7 @@
       <c r="AK46" s="59"/>
       <c r="AL46" s="60"/>
     </row>
-    <row r="47" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
@@ -4785,7 +4785,7 @@
       <c r="AK47" s="62"/>
       <c r="AL47" s="63"/>
     </row>
-    <row r="48" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
         <v>46</v>
       </c>
@@ -4824,7 +4824,7 @@
       <c r="X48" s="39"/>
       <c r="Y48" s="40"/>
     </row>
-    <row r="49" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="28" t="s">
         <v>46</v>
       </c>
@@ -4863,7 +4863,7 @@
       <c r="X49" s="42"/>
       <c r="Y49" s="43"/>
     </row>
-    <row r="51" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="79" t="s">
         <v>158</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="Z51" s="80"/>
       <c r="AA51" s="81"/>
     </row>
-    <row r="52" spans="2:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B52" s="68"/>
       <c r="C52" s="69"/>
       <c r="D52" s="69"/>
@@ -4921,7 +4921,7 @@
       <c r="Z52" s="69"/>
       <c r="AA52" s="70"/>
     </row>
-    <row r="53" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="68"/>
       <c r="C53" s="69"/>
       <c r="D53" s="69"/>
@@ -4949,7 +4949,7 @@
       <c r="Z53" s="69"/>
       <c r="AA53" s="70"/>
     </row>
-    <row r="54" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="68"/>
       <c r="C54" s="69"/>
       <c r="D54" s="69"/>
@@ -4977,7 +4977,7 @@
       <c r="Z54" s="69"/>
       <c r="AA54" s="70"/>
     </row>
-    <row r="55" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="68"/>
       <c r="C55" s="69"/>
       <c r="D55" s="69"/>
@@ -5005,7 +5005,7 @@
       <c r="Z55" s="69"/>
       <c r="AA55" s="70"/>
     </row>
-    <row r="56" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="68"/>
       <c r="C56" s="69"/>
       <c r="D56" s="69"/>
@@ -5033,7 +5033,7 @@
       <c r="Z56" s="69"/>
       <c r="AA56" s="70"/>
     </row>
-    <row r="57" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="68"/>
       <c r="C57" s="69"/>
       <c r="D57" s="69"/>
@@ -5061,7 +5061,7 @@
       <c r="Z57" s="69"/>
       <c r="AA57" s="70"/>
     </row>
-    <row r="58" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="68"/>
       <c r="C58" s="69"/>
       <c r="D58" s="69"/>
@@ -5089,7 +5089,7 @@
       <c r="Z58" s="69"/>
       <c r="AA58" s="70"/>
     </row>
-    <row r="59" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="68"/>
       <c r="C59" s="69"/>
       <c r="D59" s="69"/>
@@ -5117,7 +5117,7 @@
       <c r="Z59" s="69"/>
       <c r="AA59" s="70"/>
     </row>
-    <row r="60" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="68"/>
       <c r="C60" s="69"/>
       <c r="D60" s="69"/>
@@ -5145,7 +5145,7 @@
       <c r="Z60" s="69"/>
       <c r="AA60" s="70"/>
     </row>
-    <row r="61" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="68"/>
       <c r="C61" s="69"/>
       <c r="D61" s="69"/>
@@ -5173,7 +5173,7 @@
       <c r="Z61" s="69"/>
       <c r="AA61" s="70"/>
     </row>
-    <row r="62" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="68"/>
       <c r="C62" s="69"/>
       <c r="D62" s="69"/>
@@ -5201,7 +5201,7 @@
       <c r="Z62" s="69"/>
       <c r="AA62" s="70"/>
     </row>
-    <row r="63" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="68"/>
       <c r="C63" s="69"/>
       <c r="D63" s="69"/>
@@ -5229,7 +5229,7 @@
       <c r="Z63" s="69"/>
       <c r="AA63" s="70"/>
     </row>
-    <row r="64" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="68"/>
       <c r="C64" s="69"/>
       <c r="D64" s="69"/>
@@ -5257,7 +5257,7 @@
       <c r="Z64" s="69"/>
       <c r="AA64" s="70"/>
     </row>
-    <row r="65" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="68"/>
       <c r="C65" s="69"/>
       <c r="D65" s="69"/>
@@ -5285,7 +5285,7 @@
       <c r="Z65" s="69"/>
       <c r="AA65" s="70"/>
     </row>
-    <row r="66" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="68"/>
       <c r="C66" s="69"/>
       <c r="D66" s="69"/>
@@ -5313,7 +5313,7 @@
       <c r="Z66" s="69"/>
       <c r="AA66" s="70"/>
     </row>
-    <row r="67" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="68"/>
       <c r="C67" s="69"/>
       <c r="D67" s="69"/>
@@ -5341,7 +5341,7 @@
       <c r="Z67" s="69"/>
       <c r="AA67" s="70"/>
     </row>
-    <row r="68" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="68"/>
       <c r="C68" s="69"/>
       <c r="D68" s="69"/>
@@ -5369,7 +5369,7 @@
       <c r="Z68" s="69"/>
       <c r="AA68" s="70"/>
     </row>
-    <row r="69" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="68"/>
       <c r="C69" s="69"/>
       <c r="D69" s="69"/>
@@ -5397,7 +5397,7 @@
       <c r="Z69" s="69"/>
       <c r="AA69" s="70"/>
     </row>
-    <row r="70" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="68"/>
       <c r="C70" s="69"/>
       <c r="D70" s="69"/>
@@ -5425,7 +5425,7 @@
       <c r="Z70" s="69"/>
       <c r="AA70" s="70"/>
     </row>
-    <row r="71" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="68"/>
       <c r="C71" s="69"/>
       <c r="D71" s="69"/>
@@ -5453,7 +5453,7 @@
       <c r="Z71" s="69"/>
       <c r="AA71" s="70"/>
     </row>
-    <row r="72" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="68"/>
       <c r="C72" s="69"/>
       <c r="D72" s="69"/>
@@ -5481,7 +5481,7 @@
       <c r="Z72" s="69"/>
       <c r="AA72" s="70"/>
     </row>
-    <row r="73" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="68"/>
       <c r="C73" s="69"/>
       <c r="D73" s="69"/>
@@ -5509,7 +5509,7 @@
       <c r="Z73" s="69"/>
       <c r="AA73" s="70"/>
     </row>
-    <row r="74" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="68"/>
       <c r="C74" s="69"/>
       <c r="D74" s="69"/>
@@ -5537,7 +5537,7 @@
       <c r="Z74" s="69"/>
       <c r="AA74" s="70"/>
     </row>
-    <row r="75" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="68"/>
       <c r="C75" s="69"/>
       <c r="D75" s="69"/>
@@ -5565,7 +5565,7 @@
       <c r="Z75" s="69"/>
       <c r="AA75" s="70"/>
     </row>
-    <row r="76" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="68"/>
       <c r="C76" s="69"/>
       <c r="D76" s="69"/>
@@ -5593,7 +5593,7 @@
       <c r="Z76" s="69"/>
       <c r="AA76" s="70"/>
     </row>
-    <row r="77" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="68"/>
       <c r="C77" s="69"/>
       <c r="D77" s="69"/>
@@ -5621,7 +5621,7 @@
       <c r="Z77" s="69"/>
       <c r="AA77" s="70"/>
     </row>
-    <row r="78" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="68"/>
       <c r="C78" s="69"/>
       <c r="D78" s="69"/>
@@ -5649,7 +5649,7 @@
       <c r="Z78" s="69"/>
       <c r="AA78" s="70"/>
     </row>
-    <row r="79" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="68"/>
       <c r="C79" s="69"/>
       <c r="D79" s="69"/>
@@ -5677,7 +5677,7 @@
       <c r="Z79" s="69"/>
       <c r="AA79" s="70"/>
     </row>
-    <row r="80" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="68"/>
       <c r="C80" s="69"/>
       <c r="D80" s="69"/>
@@ -5705,7 +5705,7 @@
       <c r="Z80" s="69"/>
       <c r="AA80" s="70"/>
     </row>
-    <row r="81" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="68"/>
       <c r="C81" s="69"/>
       <c r="D81" s="69"/>
@@ -5733,7 +5733,7 @@
       <c r="Z81" s="69"/>
       <c r="AA81" s="70"/>
     </row>
-    <row r="82" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="68"/>
       <c r="C82" s="69"/>
       <c r="D82" s="69"/>
@@ -5761,7 +5761,7 @@
       <c r="Z82" s="69"/>
       <c r="AA82" s="70"/>
     </row>
-    <row r="83" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="68"/>
       <c r="C83" s="69"/>
       <c r="D83" s="69"/>
@@ -5789,7 +5789,7 @@
       <c r="Z83" s="69"/>
       <c r="AA83" s="70"/>
     </row>
-    <row r="84" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="68"/>
       <c r="C84" s="69"/>
       <c r="D84" s="69"/>
@@ -5817,7 +5817,7 @@
       <c r="Z84" s="69"/>
       <c r="AA84" s="70"/>
     </row>
-    <row r="85" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="68"/>
       <c r="C85" s="69"/>
       <c r="D85" s="69"/>
@@ -5845,7 +5845,7 @@
       <c r="Z85" s="69"/>
       <c r="AA85" s="70"/>
     </row>
-    <row r="86" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="68"/>
       <c r="C86" s="69"/>
       <c r="D86" s="69"/>
@@ -5873,7 +5873,7 @@
       <c r="Z86" s="69"/>
       <c r="AA86" s="70"/>
     </row>
-    <row r="87" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="68"/>
       <c r="C87" s="69"/>
       <c r="D87" s="69"/>
@@ -5901,7 +5901,7 @@
       <c r="Z87" s="69"/>
       <c r="AA87" s="70"/>
     </row>
-    <row r="88" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="68"/>
       <c r="C88" s="69"/>
       <c r="D88" s="69"/>
@@ -5929,7 +5929,7 @@
       <c r="Z88" s="69"/>
       <c r="AA88" s="70"/>
     </row>
-    <row r="89" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="68"/>
       <c r="C89" s="69"/>
       <c r="D89" s="69"/>
@@ -5957,7 +5957,7 @@
       <c r="Z89" s="69"/>
       <c r="AA89" s="70"/>
     </row>
-    <row r="90" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="68"/>
       <c r="C90" s="69"/>
       <c r="D90" s="69"/>
@@ -5985,7 +5985,7 @@
       <c r="Z90" s="69"/>
       <c r="AA90" s="70"/>
     </row>
-    <row r="91" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="68"/>
       <c r="C91" s="69"/>
       <c r="D91" s="69"/>
@@ -6013,7 +6013,7 @@
       <c r="Z91" s="69"/>
       <c r="AA91" s="70"/>
     </row>
-    <row r="92" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="68"/>
       <c r="C92" s="69"/>
       <c r="D92" s="69"/>
@@ -6041,7 +6041,7 @@
       <c r="Z92" s="69"/>
       <c r="AA92" s="70"/>
     </row>
-    <row r="93" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="68"/>
       <c r="C93" s="69"/>
       <c r="D93" s="69"/>
@@ -6069,7 +6069,7 @@
       <c r="Z93" s="69"/>
       <c r="AA93" s="70"/>
     </row>
-    <row r="94" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="68"/>
       <c r="C94" s="69"/>
       <c r="D94" s="69"/>
@@ -6097,7 +6097,7 @@
       <c r="Z94" s="69"/>
       <c r="AA94" s="70"/>
     </row>
-    <row r="95" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="68"/>
       <c r="C95" s="69"/>
       <c r="D95" s="69"/>
@@ -6125,7 +6125,7 @@
       <c r="Z95" s="69"/>
       <c r="AA95" s="70"/>
     </row>
-    <row r="96" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="68"/>
       <c r="C96" s="69"/>
       <c r="D96" s="69"/>
@@ -6153,7 +6153,7 @@
       <c r="Z96" s="69"/>
       <c r="AA96" s="70"/>
     </row>
-    <row r="97" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="68"/>
       <c r="C97" s="69"/>
       <c r="D97" s="69"/>
@@ -6181,7 +6181,7 @@
       <c r="Z97" s="69"/>
       <c r="AA97" s="70"/>
     </row>
-    <row r="98" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="68"/>
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
@@ -6209,7 +6209,7 @@
       <c r="Z98" s="69"/>
       <c r="AA98" s="70"/>
     </row>
-    <row r="99" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="68"/>
       <c r="C99" s="69"/>
       <c r="D99" s="69"/>
@@ -6237,7 +6237,7 @@
       <c r="Z99" s="69"/>
       <c r="AA99" s="70"/>
     </row>
-    <row r="100" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="68"/>
       <c r="C100" s="69"/>
       <c r="D100" s="69"/>
@@ -6265,7 +6265,7 @@
       <c r="Z100" s="69"/>
       <c r="AA100" s="70"/>
     </row>
-    <row r="101" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="68"/>
       <c r="C101" s="69"/>
       <c r="D101" s="69"/>
@@ -6293,7 +6293,7 @@
       <c r="Z101" s="69"/>
       <c r="AA101" s="70"/>
     </row>
-    <row r="102" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="68"/>
       <c r="C102" s="69"/>
       <c r="D102" s="69"/>
@@ -6321,7 +6321,7 @@
       <c r="Z102" s="69"/>
       <c r="AA102" s="70"/>
     </row>
-    <row r="103" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="68"/>
       <c r="C103" s="69"/>
       <c r="D103" s="69"/>
@@ -6349,7 +6349,7 @@
       <c r="Z103" s="69"/>
       <c r="AA103" s="70"/>
     </row>
-    <row r="104" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="68"/>
       <c r="C104" s="69"/>
       <c r="D104" s="69"/>
@@ -6377,7 +6377,7 @@
       <c r="Z104" s="69"/>
       <c r="AA104" s="70"/>
     </row>
-    <row r="105" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="68"/>
       <c r="C105" s="69"/>
       <c r="D105" s="69"/>
@@ -6405,7 +6405,7 @@
       <c r="Z105" s="69"/>
       <c r="AA105" s="70"/>
     </row>
-    <row r="106" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="68"/>
       <c r="C106" s="69"/>
       <c r="D106" s="69"/>
@@ -6433,7 +6433,7 @@
       <c r="Z106" s="69"/>
       <c r="AA106" s="70"/>
     </row>
-    <row r="107" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="68"/>
       <c r="C107" s="69"/>
       <c r="D107" s="69"/>
@@ -6461,7 +6461,7 @@
       <c r="Z107" s="69"/>
       <c r="AA107" s="70"/>
     </row>
-    <row r="108" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="68"/>
       <c r="C108" s="69"/>
       <c r="D108" s="69"/>
@@ -6489,7 +6489,7 @@
       <c r="Z108" s="69"/>
       <c r="AA108" s="70"/>
     </row>
-    <row r="109" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="68"/>
       <c r="C109" s="69"/>
       <c r="D109" s="69"/>
@@ -6517,7 +6517,7 @@
       <c r="Z109" s="69"/>
       <c r="AA109" s="70"/>
     </row>
-    <row r="110" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="68"/>
       <c r="C110" s="69"/>
       <c r="D110" s="69"/>
@@ -6545,7 +6545,7 @@
       <c r="Z110" s="69"/>
       <c r="AA110" s="70"/>
     </row>
-    <row r="111" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="68"/>
       <c r="C111" s="69"/>
       <c r="D111" s="69"/>
@@ -6573,7 +6573,7 @@
       <c r="Z111" s="69"/>
       <c r="AA111" s="70"/>
     </row>
-    <row r="112" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="68"/>
       <c r="C112" s="69"/>
       <c r="D112" s="69"/>
@@ -6601,7 +6601,7 @@
       <c r="Z112" s="69"/>
       <c r="AA112" s="70"/>
     </row>
-    <row r="113" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="68"/>
       <c r="C113" s="69"/>
       <c r="D113" s="69"/>
@@ -6629,7 +6629,7 @@
       <c r="Z113" s="69"/>
       <c r="AA113" s="70"/>
     </row>
-    <row r="114" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="68"/>
       <c r="C114" s="69"/>
       <c r="D114" s="69"/>
@@ -6657,7 +6657,7 @@
       <c r="Z114" s="69"/>
       <c r="AA114" s="70"/>
     </row>
-    <row r="115" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="68"/>
       <c r="C115" s="69"/>
       <c r="D115" s="69"/>
@@ -6685,7 +6685,7 @@
       <c r="Z115" s="69"/>
       <c r="AA115" s="70"/>
     </row>
-    <row r="116" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="68"/>
       <c r="C116" s="69"/>
       <c r="D116" s="69"/>
@@ -6713,7 +6713,7 @@
       <c r="Z116" s="69"/>
       <c r="AA116" s="70"/>
     </row>
-    <row r="117" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="68"/>
       <c r="C117" s="69"/>
       <c r="D117" s="69"/>
@@ -6741,7 +6741,7 @@
       <c r="Z117" s="69"/>
       <c r="AA117" s="70"/>
     </row>
-    <row r="118" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="68"/>
       <c r="C118" s="69"/>
       <c r="D118" s="69"/>
@@ -6769,7 +6769,7 @@
       <c r="Z118" s="69"/>
       <c r="AA118" s="70"/>
     </row>
-    <row r="119" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="68"/>
       <c r="C119" s="69"/>
       <c r="D119" s="69"/>
@@ -6797,7 +6797,7 @@
       <c r="Z119" s="69"/>
       <c r="AA119" s="70"/>
     </row>
-    <row r="120" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="68"/>
       <c r="C120" s="69"/>
       <c r="D120" s="69"/>
@@ -6825,7 +6825,7 @@
       <c r="Z120" s="69"/>
       <c r="AA120" s="70"/>
     </row>
-    <row r="121" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="68"/>
       <c r="C121" s="69"/>
       <c r="D121" s="69"/>
@@ -6853,7 +6853,7 @@
       <c r="Z121" s="69"/>
       <c r="AA121" s="70"/>
     </row>
-    <row r="122" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="68"/>
       <c r="C122" s="69"/>
       <c r="D122" s="69"/>
@@ -6881,7 +6881,7 @@
       <c r="Z122" s="69"/>
       <c r="AA122" s="70"/>
     </row>
-    <row r="123" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="68"/>
       <c r="C123" s="69"/>
       <c r="D123" s="69"/>
@@ -6909,7 +6909,7 @@
       <c r="Z123" s="69"/>
       <c r="AA123" s="70"/>
     </row>
-    <row r="124" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="68"/>
       <c r="C124" s="69"/>
       <c r="D124" s="69"/>
@@ -6937,7 +6937,7 @@
       <c r="Z124" s="69"/>
       <c r="AA124" s="70"/>
     </row>
-    <row r="125" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="68"/>
       <c r="C125" s="69"/>
       <c r="D125" s="69"/>
@@ -6965,7 +6965,7 @@
       <c r="Z125" s="69"/>
       <c r="AA125" s="70"/>
     </row>
-    <row r="126" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="68"/>
       <c r="C126" s="69"/>
       <c r="D126" s="69"/>
@@ -6993,7 +6993,7 @@
       <c r="Z126" s="69"/>
       <c r="AA126" s="70"/>
     </row>
-    <row r="127" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="68"/>
       <c r="C127" s="69"/>
       <c r="D127" s="69"/>
@@ -7021,7 +7021,7 @@
       <c r="Z127" s="69"/>
       <c r="AA127" s="70"/>
     </row>
-    <row r="128" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="68"/>
       <c r="C128" s="69"/>
       <c r="D128" s="69"/>
@@ -7049,7 +7049,7 @@
       <c r="Z128" s="69"/>
       <c r="AA128" s="70"/>
     </row>
-    <row r="129" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="68"/>
       <c r="C129" s="69"/>
       <c r="D129" s="69"/>
@@ -7077,7 +7077,7 @@
       <c r="Z129" s="69"/>
       <c r="AA129" s="70"/>
     </row>
-    <row r="130" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="68"/>
       <c r="C130" s="69"/>
       <c r="D130" s="69"/>
@@ -7105,7 +7105,7 @@
       <c r="Z130" s="69"/>
       <c r="AA130" s="70"/>
     </row>
-    <row r="131" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="68"/>
       <c r="C131" s="69"/>
       <c r="D131" s="69"/>
@@ -7133,7 +7133,7 @@
       <c r="Z131" s="69"/>
       <c r="AA131" s="70"/>
     </row>
-    <row r="132" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="68"/>
       <c r="C132" s="69"/>
       <c r="D132" s="69"/>
@@ -7161,7 +7161,7 @@
       <c r="Z132" s="69"/>
       <c r="AA132" s="70"/>
     </row>
-    <row r="133" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="68"/>
       <c r="C133" s="69"/>
       <c r="D133" s="69"/>
@@ -7189,7 +7189,7 @@
       <c r="Z133" s="69"/>
       <c r="AA133" s="70"/>
     </row>
-    <row r="134" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="68"/>
       <c r="C134" s="69"/>
       <c r="D134" s="69"/>
@@ -7217,7 +7217,7 @@
       <c r="Z134" s="69"/>
       <c r="AA134" s="70"/>
     </row>
-    <row r="135" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="68"/>
       <c r="C135" s="69"/>
       <c r="D135" s="69"/>
@@ -7245,7 +7245,7 @@
       <c r="Z135" s="69"/>
       <c r="AA135" s="70"/>
     </row>
-    <row r="136" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="68"/>
       <c r="C136" s="69"/>
       <c r="D136" s="69"/>
@@ -7273,7 +7273,7 @@
       <c r="Z136" s="69"/>
       <c r="AA136" s="70"/>
     </row>
-    <row r="137" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="68"/>
       <c r="C137" s="69"/>
       <c r="D137" s="69"/>
@@ -7301,7 +7301,7 @@
       <c r="Z137" s="69"/>
       <c r="AA137" s="70"/>
     </row>
-    <row r="138" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="68"/>
       <c r="C138" s="69"/>
       <c r="D138" s="69"/>
@@ -7329,7 +7329,7 @@
       <c r="Z138" s="69"/>
       <c r="AA138" s="70"/>
     </row>
-    <row r="139" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="68"/>
       <c r="C139" s="69"/>
       <c r="D139" s="69"/>
@@ -7357,7 +7357,7 @@
       <c r="Z139" s="69"/>
       <c r="AA139" s="70"/>
     </row>
-    <row r="140" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="68"/>
       <c r="C140" s="69"/>
       <c r="D140" s="69"/>
@@ -7385,7 +7385,7 @@
       <c r="Z140" s="69"/>
       <c r="AA140" s="70"/>
     </row>
-    <row r="141" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="68"/>
       <c r="C141" s="69"/>
       <c r="D141" s="69"/>
@@ -7413,7 +7413,7 @@
       <c r="Z141" s="69"/>
       <c r="AA141" s="70"/>
     </row>
-    <row r="142" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="68"/>
       <c r="C142" s="69"/>
       <c r="D142" s="69"/>
@@ -7441,7 +7441,7 @@
       <c r="Z142" s="69"/>
       <c r="AA142" s="70"/>
     </row>
-    <row r="143" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="68"/>
       <c r="C143" s="69"/>
       <c r="D143" s="69"/>
@@ -7469,7 +7469,7 @@
       <c r="Z143" s="69"/>
       <c r="AA143" s="70"/>
     </row>
-    <row r="144" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="68"/>
       <c r="C144" s="69"/>
       <c r="D144" s="69"/>
@@ -7497,7 +7497,7 @@
       <c r="Z144" s="69"/>
       <c r="AA144" s="70"/>
     </row>
-    <row r="145" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="68"/>
       <c r="C145" s="69"/>
       <c r="D145" s="69"/>
@@ -7525,7 +7525,7 @@
       <c r="Z145" s="69"/>
       <c r="AA145" s="70"/>
     </row>
-    <row r="146" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="68"/>
       <c r="C146" s="69"/>
       <c r="D146" s="69"/>
@@ -7553,7 +7553,7 @@
       <c r="Z146" s="69"/>
       <c r="AA146" s="70"/>
     </row>
-    <row r="147" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="68"/>
       <c r="C147" s="69"/>
       <c r="D147" s="69"/>
@@ -7581,7 +7581,7 @@
       <c r="Z147" s="69"/>
       <c r="AA147" s="70"/>
     </row>
-    <row r="148" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="68"/>
       <c r="C148" s="69"/>
       <c r="D148" s="69"/>
@@ -7609,7 +7609,7 @@
       <c r="Z148" s="69"/>
       <c r="AA148" s="70"/>
     </row>
-    <row r="149" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="68"/>
       <c r="C149" s="69"/>
       <c r="D149" s="69"/>
@@ -7637,7 +7637,7 @@
       <c r="Z149" s="69"/>
       <c r="AA149" s="70"/>
     </row>
-    <row r="150" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="68"/>
       <c r="C150" s="69"/>
       <c r="D150" s="69"/>
@@ -7665,7 +7665,7 @@
       <c r="Z150" s="69"/>
       <c r="AA150" s="70"/>
     </row>
-    <row r="151" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="68"/>
       <c r="C151" s="69"/>
       <c r="D151" s="69"/>
@@ -7693,7 +7693,7 @@
       <c r="Z151" s="69"/>
       <c r="AA151" s="70"/>
     </row>
-    <row r="152" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="68"/>
       <c r="C152" s="69"/>
       <c r="D152" s="69"/>
@@ -7721,7 +7721,7 @@
       <c r="Z152" s="69"/>
       <c r="AA152" s="70"/>
     </row>
-    <row r="153" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="68"/>
       <c r="C153" s="69"/>
       <c r="D153" s="69"/>
@@ -7749,7 +7749,7 @@
       <c r="Z153" s="69"/>
       <c r="AA153" s="70"/>
     </row>
-    <row r="154" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="68"/>
       <c r="C154" s="69"/>
       <c r="D154" s="69"/>
@@ -7777,7 +7777,7 @@
       <c r="Z154" s="69"/>
       <c r="AA154" s="70"/>
     </row>
-    <row r="155" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="68"/>
       <c r="C155" s="69"/>
       <c r="D155" s="69"/>
@@ -7805,7 +7805,7 @@
       <c r="Z155" s="69"/>
       <c r="AA155" s="70"/>
     </row>
-    <row r="156" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="68"/>
       <c r="C156" s="69"/>
       <c r="D156" s="69"/>
@@ -7833,7 +7833,7 @@
       <c r="Z156" s="69"/>
       <c r="AA156" s="70"/>
     </row>
-    <row r="157" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="68"/>
       <c r="C157" s="69"/>
       <c r="D157" s="69"/>
@@ -7861,7 +7861,7 @@
       <c r="Z157" s="69"/>
       <c r="AA157" s="70"/>
     </row>
-    <row r="158" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="71"/>
       <c r="C158" s="72"/>
       <c r="D158" s="72"/>
@@ -7904,79 +7904,79 @@
     <mergeCell ref="AA18:AL18"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:F27 B31:F49">
-    <cfRule type="expression" dxfId="23" priority="977">
-      <formula>$B9=$M$9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="966">
+    <cfRule type="expression" dxfId="23" priority="966">
       <formula>$B9=$M$15</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="967">
+    <cfRule type="expression" dxfId="22" priority="967">
       <formula>$B9=$M$13</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="968">
+    <cfRule type="expression" dxfId="21" priority="968">
       <formula>$B9=$M$18</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="969">
+    <cfRule type="expression" dxfId="20" priority="969">
       <formula>$B9=$M$14</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="970">
+    <cfRule type="expression" dxfId="19" priority="970">
       <formula>$B9=$M$19</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="971">
+    <cfRule type="expression" dxfId="18" priority="971">
       <formula>$B9=$M$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="972">
+    <cfRule type="expression" dxfId="17" priority="972">
       <formula>$B9=$M$16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="973">
+    <cfRule type="expression" dxfId="16" priority="973">
       <formula>$B9=$M$20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="974">
+    <cfRule type="expression" dxfId="15" priority="974">
       <formula>$B9=$M$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="975">
+    <cfRule type="expression" dxfId="14" priority="975">
       <formula>$B9=$M$17</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="976">
+    <cfRule type="expression" dxfId="13" priority="976">
       <formula>$B9=$M$11</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="977">
+      <formula>$B9=$M$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:K27 G31:K49">
-    <cfRule type="expression" dxfId="11" priority="955">
+    <cfRule type="expression" dxfId="11" priority="954">
+      <formula>$K9=$M$15</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="955">
       <formula>$K9=$M$13</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="956">
+    <cfRule type="expression" dxfId="9" priority="956">
       <formula>$K9=$M$18</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="957">
+    <cfRule type="expression" dxfId="8" priority="957">
       <formula>$K9=$M$14</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="958">
+    <cfRule type="expression" dxfId="7" priority="958">
       <formula>$K9=$M$19</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="959">
+    <cfRule type="expression" dxfId="6" priority="959">
       <formula>$K9=$M$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="960">
+    <cfRule type="expression" dxfId="5" priority="960">
       <formula>$K9=$M$16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="961">
+    <cfRule type="expression" dxfId="4" priority="961">
       <formula>$K9=$M$20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="962">
+    <cfRule type="expression" dxfId="3" priority="962">
       <formula>$K9=$M$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="963">
+    <cfRule type="expression" dxfId="2" priority="963">
       <formula>$K9=$M$17</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="964">
+    <cfRule type="expression" dxfId="1" priority="964">
       <formula>$K9=$M$11</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="965">
+    <cfRule type="expression" dxfId="0" priority="965">
       <formula>$K9=$M$9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="954">
-      <formula>$K9=$M$15</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -8001,20 +8001,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AECF287-01B5-9A49-98CA-7F36E611FCB7}">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>159</v>
       </c>
@@ -8035,7 +8037,7 @@
       </c>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>165</v>
       </c>
@@ -8058,7 +8060,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>171</v>
       </c>
@@ -8079,7 +8081,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>175</v>
       </c>
@@ -8102,7 +8104,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>180</v>
       </c>
@@ -8126,7 +8128,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>185</v>
       </c>
@@ -8147,7 +8149,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>189</v>
       </c>
@@ -8161,7 +8163,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>191</v>
       </c>
@@ -8175,7 +8177,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>193</v>
       </c>
@@ -8189,7 +8191,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>195</v>
       </c>
@@ -8204,7 +8206,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>198</v>
       </c>
@@ -8212,7 +8214,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>200</v>
       </c>
@@ -8228,7 +8230,7 @@
         <v>0.12217304763960309</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="16" t="s">
         <v>201</v>
       </c>
@@ -8242,7 +8244,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>205</v>
       </c>
@@ -8267,7 +8269,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>208</v>
       </c>
@@ -8296,7 +8298,7 @@
         <v>0.25000000000000006</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
         <v>210</v>
       </c>

</xml_diff>